<commit_message>
Cleaned up disciplinary actions on all 2016 HOU home games
</commit_message>
<xml_diff>
--- a/source/excel/nwsl-2016/nwsl-2016-hou-fckc-061916.xlsx
+++ b/source/excel/nwsl-2016/nwsl-2016-hou-fckc-061916.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alfredo/Desktop/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="460" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1204,8 +1204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T1424"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView tabSelected="1" topLeftCell="F1347" workbookViewId="0">
+      <selection activeCell="N1353" sqref="N1353"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>